<commit_message>
fixed the main issue: delete microsoft python, run scrapling install on the bootstrapper. Maybe also add an uninstall statement if it fails once? Up to you caleb
</commit_message>
<xml_diff>
--- a/scraplingAdaptationHana/wholefoods/wholefoods_price_compare/wholefoods_pc.xlsx
+++ b/scraplingAdaptationHana/wholefoods/wholefoods_price_compare/wholefoods_pc.xlsx
@@ -718,7 +718,7 @@
       <c r="J4" s="6" t="inlineStr"/>
       <c r="K4" s="6" t="inlineStr">
         <is>
-          <t>Pinot Bianco, 750 ML</t>
+          <t>Chardonnay, 750 ML</t>
         </is>
       </c>
       <c r="L4" s="7" t="n">
@@ -768,11 +768,11 @@
       <c r="J5" s="6" t="inlineStr"/>
       <c r="K5" s="6" t="inlineStr">
         <is>
-          <t>Cranberry Wensleydale</t>
+          <t>Blueberry Wensleydale</t>
         </is>
       </c>
       <c r="L5" s="7" t="n">
-        <v>44.89795918367347</v>
+        <v>40.81632653061224</v>
       </c>
     </row>
     <row r="6">
@@ -818,11 +818,11 @@
       <c r="J6" s="6" t="inlineStr"/>
       <c r="K6" s="6" t="inlineStr">
         <is>
-          <t>Peppermint Sponge Floss, 55 YD</t>
+          <t>Cremant Rose, 750 ML</t>
         </is>
       </c>
       <c r="L6" s="7" t="n">
-        <v>40</v>
+        <v>43.13725490196079</v>
       </c>
     </row>
     <row r="7">
@@ -868,11 +868,11 @@
       <c r="J7" s="6" t="inlineStr"/>
       <c r="K7" s="6" t="inlineStr">
         <is>
-          <t>Moses Sleeper</t>
+          <t>Imperial Rioja Reserva, 750 ML</t>
         </is>
       </c>
       <c r="L7" s="7" t="n">
-        <v>41.66666666666666</v>
+        <v>42.30769230769231</v>
       </c>
     </row>
     <row r="8">
@@ -1018,11 +1018,11 @@
       <c r="J10" s="6" t="inlineStr"/>
       <c r="K10" s="6" t="inlineStr">
         <is>
-          <t>Brown Asian Pear</t>
+          <t>Red Wine Vinegar, 16.9 FZ</t>
         </is>
       </c>
       <c r="L10" s="7" t="n">
-        <v>43.90243902439025</v>
+        <v>42.10526315789474</v>
       </c>
     </row>
     <row r="11">
@@ -1068,11 +1068,11 @@
       <c r="J11" s="6" t="inlineStr"/>
       <c r="K11" s="6" t="inlineStr">
         <is>
-          <t>Stone Ground White Grits, 24 OZ</t>
+          <t>Vinegar Rice Premium, 10 FZ</t>
         </is>
       </c>
       <c r="L11" s="7" t="n">
-        <v>38.70967741935484</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12">
@@ -1118,11 +1118,11 @@
       <c r="J12" s="6" t="inlineStr"/>
       <c r="K12" s="6" t="inlineStr">
         <is>
-          <t>Stone Ground White Grits, 24 OZ</t>
+          <t>Vinegar Rice Premium, 10 FZ</t>
         </is>
       </c>
       <c r="L12" s="7" t="n">
-        <v>38.70967741935484</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13">
@@ -1318,11 +1318,11 @@
       <c r="J16" s="6" t="inlineStr"/>
       <c r="K16" s="6" t="inlineStr">
         <is>
-          <t>Apple Juice, 52 FZ</t>
+          <t>Apple Juice, 64 FZ</t>
         </is>
       </c>
       <c r="L16" s="7" t="n">
-        <v>39.02439024390244</v>
+        <v>36.36363636363637</v>
       </c>
     </row>
     <row r="17">
@@ -1418,11 +1418,11 @@
       <c r="J18" s="6" t="inlineStr"/>
       <c r="K18" s="6" t="inlineStr">
         <is>
-          <t>Comte</t>
+          <t>Pecorino Romano</t>
         </is>
       </c>
       <c r="L18" s="7" t="n">
-        <v>43.47826086956522</v>
+        <v>34.48275862068965</v>
       </c>
     </row>
     <row r="19">
@@ -1468,11 +1468,11 @@
       <c r="J19" s="6" t="inlineStr"/>
       <c r="K19" s="6" t="inlineStr">
         <is>
-          <t>Comte</t>
+          <t>Pecorino Romano</t>
         </is>
       </c>
       <c r="L19" s="7" t="n">
-        <v>43.47826086956522</v>
+        <v>34.48275862068965</v>
       </c>
     </row>
     <row r="20">
@@ -1518,11 +1518,11 @@
       <c r="J20" s="6" t="inlineStr"/>
       <c r="K20" s="6" t="inlineStr">
         <is>
-          <t>Roma Tomato</t>
+          <t>Cinnamon Toast Cereal, 9 OZ</t>
         </is>
       </c>
       <c r="L20" s="7" t="n">
-        <v>41.02564102564103</v>
+        <v>48.38709677419355</v>
       </c>
     </row>
     <row r="21">
@@ -1568,11 +1568,11 @@
       <c r="J21" s="6" t="inlineStr"/>
       <c r="K21" s="6" t="inlineStr">
         <is>
-          <t>Cambozola Black Label</t>
+          <t>Brut, 750 ML</t>
         </is>
       </c>
       <c r="L21" s="7" t="n">
-        <v>36</v>
+        <v>35.55555555555556</v>
       </c>
     </row>
     <row r="22">
@@ -1718,11 +1718,11 @@
       <c r="J24" s="6" t="inlineStr"/>
       <c r="K24" s="6" t="inlineStr">
         <is>
-          <t>Rose, 750 ML</t>
+          <t>Taleggio</t>
         </is>
       </c>
       <c r="L24" s="7" t="n">
-        <v>42.42424242424242</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25">
@@ -1768,11 +1768,11 @@
       <c r="J25" s="6" t="inlineStr"/>
       <c r="K25" s="6" t="inlineStr">
         <is>
-          <t>Rose, 750 ML</t>
+          <t>Taleggio</t>
         </is>
       </c>
       <c r="L25" s="7" t="n">
-        <v>42.42424242424242</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26">

</xml_diff>